<commit_message>
Add data for 2021-08-21
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,17 +660,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-12)</t>
+          <t>August (through 08-13)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="n">
         <v>21</v>
@@ -679,10 +679,10 @@
         <v>16</v>
       </c>
       <c r="G9" t="n">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H9" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -692,13 +692,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C10" t="n">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D10" t="n">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E10" t="n">
         <v>446</v>
@@ -707,10 +707,10 @@
         <v>320</v>
       </c>
       <c r="G10" t="n">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="H10" t="n">
-        <v>987</v>
+        <v>990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-22
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-13)</t>
+          <t>August (through 08-14)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D9" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E9" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F9" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G9" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H9" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C10" t="n">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D10" t="n">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="E10" t="n">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F10" t="n">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="G10" t="n">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H10" t="n">
-        <v>990</v>
+        <v>992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-23
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-14)</t>
+          <t>August (through 08-15)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E9" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" t="n">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H9" t="n">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C10" t="n">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D10" t="n">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="E10" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F10" t="n">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G10" t="n">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="H10" t="n">
-        <v>992</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-24
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-15)</t>
+          <t>August (through 08-16)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D9" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E9" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F9" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" t="n">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="H9" t="n">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C10" t="n">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="D10" t="n">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="E10" t="n">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="F10" t="n">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G10" t="n">
-        <v>714</v>
+        <v>722</v>
       </c>
       <c r="H10" t="n">
-        <v>1000</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-25
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -654,35 +654,35 @@
         <v>149</v>
       </c>
       <c r="H8" t="n">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-16)</t>
+          <t>August (through 08-17)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="n">
         <v>42</v>
       </c>
       <c r="D9" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E9" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G9" t="n">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="H9" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
@@ -692,22 +692,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C10" t="n">
         <v>344</v>
       </c>
       <c r="D10" t="n">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="E10" t="n">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F10" t="n">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G10" t="n">
-        <v>722</v>
+        <v>732</v>
       </c>
       <c r="H10" t="n">
         <v>1006</v>

</xml_diff>

<commit_message>
Add data for 2021-08-26
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,7 +660,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-17)</t>
+          <t>August (through 08-18)</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -670,19 +670,19 @@
         <v>42</v>
       </c>
       <c r="D9" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E9" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" t="n">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H9" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
@@ -698,19 +698,19 @@
         <v>344</v>
       </c>
       <c r="D10" t="n">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="E10" t="n">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F10" t="n">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G10" t="n">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="H10" t="n">
-        <v>1006</v>
+        <v>1008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-27
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -598,7 +598,7 @@
         <v>96</v>
       </c>
       <c r="H6" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7">
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-18)</t>
+          <t>August (through 08-19)</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D9" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E9" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F9" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G9" t="n">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H9" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10">
@@ -695,22 +695,22 @@
         <v>182</v>
       </c>
       <c r="C10" t="n">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="D10" t="n">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E10" t="n">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F10" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G10" t="n">
-        <v>736</v>
+        <v>743</v>
       </c>
       <c r="H10" t="n">
-        <v>1008</v>
+        <v>1011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-28
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -626,7 +626,7 @@
         <v>114</v>
       </c>
       <c r="H7" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8">
@@ -660,17 +660,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-19)</t>
+          <t>August (through 08-20)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" t="n">
         <v>31</v>
@@ -679,10 +679,10 @@
         <v>27</v>
       </c>
       <c r="G9" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H9" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10">
@@ -692,13 +692,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C10" t="n">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D10" t="n">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="E10" t="n">
         <v>456</v>
@@ -707,10 +707,10 @@
         <v>331</v>
       </c>
       <c r="G10" t="n">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="H10" t="n">
-        <v>1011</v>
+        <v>1017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-29
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -654,35 +654,35 @@
         <v>149</v>
       </c>
       <c r="H8" t="n">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-20)</t>
+          <t>August (through 08-21)</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>22</v>
       </c>
       <c r="C9" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D9" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E9" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" t="n">
         <v>27</v>
       </c>
       <c r="G9" t="n">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="H9" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
@@ -695,22 +695,22 @@
         <v>184</v>
       </c>
       <c r="C10" t="n">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D10" t="n">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E10" t="n">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F10" t="n">
         <v>331</v>
       </c>
       <c r="G10" t="n">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="H10" t="n">
-        <v>1017</v>
+        <v>1020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-30
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-21)</t>
+          <t>August (through 08-22)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E9" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F9" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G9" t="n">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H9" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C10" t="n">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D10" t="n">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="E10" t="n">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="F10" t="n">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G10" t="n">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="H10" t="n">
-        <v>1020</v>
+        <v>1023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-08-31
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -570,7 +570,7 @@
         <v>64</v>
       </c>
       <c r="H5" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-22)</t>
+          <t>August (through 08-23)</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E9" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H9" t="n">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
@@ -695,22 +695,22 @@
         <v>187</v>
       </c>
       <c r="C10" t="n">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D10" t="n">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="E10" t="n">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F10" t="n">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="G10" t="n">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="H10" t="n">
-        <v>1023</v>
+        <v>1033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-01
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-23)</t>
+          <t>August (through 08-24)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D9" t="n">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E9" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F9" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H9" t="n">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C10" t="n">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="D10" t="n">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="E10" t="n">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="F10" t="n">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G10" t="n">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="H10" t="n">
-        <v>1033</v>
+        <v>1036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-02
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -598,7 +598,7 @@
         <v>96</v>
       </c>
       <c r="H6" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7">
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-24)</t>
+          <t>August (through 08-25)</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>26</v>
       </c>
       <c r="C9" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D9" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E9" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F9" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G9" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H9" t="n">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10">
@@ -695,22 +695,22 @@
         <v>188</v>
       </c>
       <c r="C10" t="n">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="D10" t="n">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="E10" t="n">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="F10" t="n">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="G10" t="n">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="H10" t="n">
-        <v>1036</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-03
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-25)</t>
+          <t>August (through 08-26)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D9" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E9" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F9" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" t="n">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H9" t="n">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C10" t="n">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D10" t="n">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="E10" t="n">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="F10" t="n">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G10" t="n">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="H10" t="n">
-        <v>1038</v>
+        <v>1046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-04
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-26)</t>
+          <t>August (through 08-27)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D9" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E9" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F9" t="n">
         <v>38</v>
       </c>
       <c r="G9" t="n">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H9" t="n">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C10" t="n">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D10" t="n">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="E10" t="n">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="F10" t="n">
         <v>342</v>
       </c>
       <c r="G10" t="n">
-        <v>766</v>
+        <v>773</v>
       </c>
       <c r="H10" t="n">
-        <v>1046</v>
+        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-05
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-27)</t>
+          <t>August (through 08-28)</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>28</v>
       </c>
       <c r="C9" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E9" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F9" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G9" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H9" t="n">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10">
@@ -695,22 +695,22 @@
         <v>190</v>
       </c>
       <c r="C10" t="n">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D10" t="n">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="E10" t="n">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F10" t="n">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="G10" t="n">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="H10" t="n">
-        <v>1050</v>
+        <v>1058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-06
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -626,7 +626,7 @@
         <v>114</v>
       </c>
       <c r="H7" t="n">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8">
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-28)</t>
+          <t>August (through 08-29)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" t="n">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D9" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F9" t="n">
         <v>42</v>
       </c>
       <c r="G9" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H9" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C10" t="n">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="D10" t="n">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E10" t="n">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="F10" t="n">
         <v>346</v>
       </c>
       <c r="G10" t="n">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="H10" t="n">
-        <v>1058</v>
+        <v>1061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-07
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,29 +660,29 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-29)</t>
+          <t>August (through 08-30)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D9" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E9" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F9" t="n">
         <v>42</v>
       </c>
       <c r="G9" t="n">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H9" t="n">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +692,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C10" t="n">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D10" t="n">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E10" t="n">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F10" t="n">
         <v>346</v>
       </c>
       <c r="G10" t="n">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="H10" t="n">
-        <v>1061</v>
+        <v>1065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-08
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -660,14 +660,14 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-30)</t>
+          <t>August (through 08-31)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D9" t="n">
         <v>86</v>
@@ -676,13 +676,13 @@
         <v>65</v>
       </c>
       <c r="F9" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G9" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H9" t="n">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
@@ -692,10 +692,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C10" t="n">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D10" t="n">
         <v>551</v>
@@ -704,13 +704,13 @@
         <v>490</v>
       </c>
       <c r="F10" t="n">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G10" t="n">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="H10" t="n">
-        <v>1065</v>
+        <v>1069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-09
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,7 +660,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>August (through 08-31)</t>
+          <t>August</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -682,35 +682,61 @@
         <v>163</v>
       </c>
       <c r="H9" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
+          <t>September (through 09-01)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B11" t="n">
         <v>194</v>
       </c>
-      <c r="C10" t="n">
-        <v>381</v>
-      </c>
-      <c r="D10" t="n">
-        <v>551</v>
-      </c>
-      <c r="E10" t="n">
-        <v>490</v>
-      </c>
-      <c r="F10" t="n">
-        <v>349</v>
-      </c>
-      <c r="G10" t="n">
-        <v>784</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1069</v>
+      <c r="C11" t="n">
+        <v>382</v>
+      </c>
+      <c r="D11" t="n">
+        <v>553</v>
+      </c>
+      <c r="E11" t="n">
+        <v>492</v>
+      </c>
+      <c r="F11" t="n">
+        <v>357</v>
+      </c>
+      <c r="G11" t="n">
+        <v>787</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-10
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -688,7 +688,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>September (through 09-01)</t>
+          <t>September (through 09-02)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -696,19 +696,19 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
         <v>8</v>
       </c>
       <c r="G10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -724,19 +724,19 @@
         <v>382</v>
       </c>
       <c r="D11" t="n">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="E11" t="n">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F11" t="n">
         <v>357</v>
       </c>
       <c r="G11" t="n">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="H11" t="n">
-        <v>1076</v>
+        <v>1078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-11
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -688,27 +688,29 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>September (through 09-02)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+          <t>September (through 09-03)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11</v>
+      </c>
+      <c r="G10" t="n">
         <v>8</v>
       </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" t="n">
-        <v>8</v>
-      </c>
-      <c r="G10" t="n">
-        <v>5</v>
-      </c>
       <c r="H10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -718,25 +720,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C11" t="n">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D11" t="n">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="E11" t="n">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F11" t="n">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="G11" t="n">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="H11" t="n">
-        <v>1078</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-12
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -682,35 +682,35 @@
         <v>163</v>
       </c>
       <c r="H9" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>September (through 09-03)</t>
+          <t>September (through 09-04)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
         <v>11</v>
       </c>
       <c r="G10" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H10" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -720,25 +720,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C11" t="n">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D11" t="n">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E11" t="n">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F11" t="n">
         <v>360</v>
       </c>
       <c r="G11" t="n">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="H11" t="n">
-        <v>1080</v>
+        <v>1088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-13
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -688,29 +688,29 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>September (through 09-04)</t>
+          <t>September (through 09-05)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
         <v>11</v>
       </c>
       <c r="G10" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H10" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -720,25 +720,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C11" t="n">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D11" t="n">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E11" t="n">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F11" t="n">
         <v>360</v>
       </c>
       <c r="G11" t="n">
-        <v>795</v>
+        <v>802</v>
       </c>
       <c r="H11" t="n">
-        <v>1088</v>
+        <v>1093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-14
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -688,29 +688,29 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>September (through 09-05)</t>
+          <t>September (through 09-06)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D10" t="n">
         <v>14</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F10" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G10" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H10" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -720,25 +720,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C11" t="n">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D11" t="n">
         <v>565</v>
       </c>
       <c r="E11" t="n">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="F11" t="n">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G11" t="n">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="H11" t="n">
-        <v>1093</v>
+        <v>1097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-15
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-06" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-07" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-06)</t>
+    <t>September (through 09-07)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H10">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C11">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D11">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="E11">
         <v>499</v>
       </c>
       <c r="F11">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="G11">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="H11">
-        <v>1097</v>
+        <v>1099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-16
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-07" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-08" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-07)</t>
+    <t>September (through 09-08)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>13</v>
       </c>
       <c r="D10">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G10">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H10">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C11">
         <v>394</v>
       </c>
       <c r="D11">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E11">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F11">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="G11">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="H11">
-        <v>1099</v>
+        <v>1101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-17
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-08" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-09" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-08)</t>
+    <t>September (through 09-09)</t>
   </si>
   <si>
     <t>Total</t>
@@ -662,22 +662,22 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H10">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -688,22 +688,22 @@
         <v>202</v>
       </c>
       <c r="C11">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D11">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="E11">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="F11">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G11">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H11">
-        <v>1101</v>
+        <v>1107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-18
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-09" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-10" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-09)</t>
+    <t>September (through 09-10)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
         <v>15</v>
       </c>
-      <c r="D10">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <v>14</v>
-      </c>
       <c r="F10">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G10">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H10">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C11">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D11">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="E11">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F11">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="G11">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="H11">
-        <v>1107</v>
+        <v>1114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-19
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-10" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-11" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-10)</t>
+    <t>September (through 09-11)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10">
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
         <v>25</v>
       </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
-      <c r="F10">
-        <v>23</v>
-      </c>
       <c r="G10">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H10">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C11">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D11">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E11">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="F11">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G11">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="H11">
-        <v>1114</v>
+        <v>1124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-20
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-11" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-12" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-11)</t>
+    <t>September (through 09-12)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F10">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G10">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H10">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C11">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D11">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="E11">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F11">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G11">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="H11">
-        <v>1124</v>
+        <v>1129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-21
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-12" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-13" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-12)</t>
+    <t>September (through 09-13)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>26</v>
+      </c>
+      <c r="F10">
         <v>30</v>
       </c>
-      <c r="E10">
-        <v>24</v>
-      </c>
-      <c r="F10">
-        <v>28</v>
-      </c>
       <c r="G10">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H10">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C11">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D11">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E11">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="F11">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G11">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="H11">
-        <v>1129</v>
+        <v>1137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-22
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-13" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-14" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-13)</t>
+    <t>September (through 09-14)</t>
   </si>
   <si>
     <t>Total</t>
@@ -521,7 +521,7 @@
         <v>57</v>
       </c>
       <c r="H4">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10">
         <v>30</v>
       </c>
       <c r="G10">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H10">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C11">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D11">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E11">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="F11">
         <v>379</v>
       </c>
       <c r="G11">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="H11">
-        <v>1137</v>
+        <v>1140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-23
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-14" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-15" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-14)</t>
+    <t>September (through 09-15)</t>
   </si>
   <si>
     <t>Total</t>
@@ -662,22 +662,22 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G10">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H10">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -688,22 +688,22 @@
         <v>209</v>
       </c>
       <c r="C11">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D11">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E11">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F11">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="G11">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="H11">
-        <v>1140</v>
+        <v>1146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-24
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-15" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-16" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-15)</t>
+    <t>September (through 09-16)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G10">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H10">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C11">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D11">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="E11">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F11">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="G11">
-        <v>841</v>
+        <v>845</v>
       </c>
       <c r="H11">
-        <v>1146</v>
+        <v>1150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-25
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-16" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-17" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-16)</t>
+    <t>September (through 09-17)</t>
   </si>
   <si>
     <t>Total</t>
@@ -662,22 +662,22 @@
         <v>17</v>
       </c>
       <c r="C10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>40</v>
       </c>
       <c r="E10">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G10">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H10">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -688,22 +688,22 @@
         <v>211</v>
       </c>
       <c r="C11">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D11">
         <v>591</v>
       </c>
       <c r="E11">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="F11">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="G11">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="H11">
-        <v>1150</v>
+        <v>1157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-26
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-17" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-18" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-17)</t>
+    <t>September (through 09-18)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H10">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C11">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D11">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E11">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="F11">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G11">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="H11">
-        <v>1157</v>
+        <v>1165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-27
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-18" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-19" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-18)</t>
+    <t>September (through 09-19)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E10">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G10">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H10">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C11">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D11">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E11">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="F11">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="G11">
-        <v>850</v>
+        <v>858</v>
       </c>
       <c r="H11">
-        <v>1165</v>
+        <v>1179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-28
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-19" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-20" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-19)</t>
+    <t>September (through 09-20)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>34</v>
       </c>
       <c r="D10">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F10">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H10">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C11">
         <v>415</v>
       </c>
       <c r="D11">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E11">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F11">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G11">
-        <v>858</v>
+        <v>864</v>
       </c>
       <c r="H11">
-        <v>1179</v>
+        <v>1191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2021-09-29
</commit_message>
<xml_diff>
--- a/output/excel/carjacking-by-month-yoy-latest.xlsx
+++ b/output/excel/carjacking-by-month-yoy-latest.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Through 2021-09-20" sheetId="1" r:id="rId1"/>
+    <sheet name="Through 2021-09-21" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
     <t>August</t>
   </si>
   <si>
-    <t>September (through 09-20)</t>
+    <t>September (through 09-21)</t>
   </si>
   <si>
     <t>Total</t>
@@ -659,25 +659,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>34</v>
       </c>
       <c r="D10">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F10">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G10">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H10">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -685,25 +685,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C11">
         <v>415</v>
       </c>
       <c r="D11">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="E11">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F11">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="G11">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="H11">
-        <v>1191</v>
+        <v>1197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>